<commit_message>
Add option for true false
</commit_message>
<xml_diff>
--- a/Validation/common_judges/average_Cohen_ALL.xlsx
+++ b/Validation/common_judges/average_Cohen_ALL.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
-  <si>
-    <t>lena</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>cvai</t>
   </si>
@@ -381,13 +378,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -421,11 +418,8 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -462,11 +456,8 @@
       <c r="L2">
         <v>0.6687886378192066</v>
       </c>
-      <c r="M2">
-        <v>0.6129792080926055</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -503,11 +494,8 @@
       <c r="L3">
         <v>0.7443044622113346</v>
       </c>
-      <c r="M3">
-        <v>0.7873734238037797</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -544,11 +532,8 @@
       <c r="L4">
         <v>0.7310548694647117</v>
       </c>
-      <c r="M4">
-        <v>0.7998627534245834</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -585,11 +570,8 @@
       <c r="L5">
         <v>0.5255208821787767</v>
       </c>
-      <c r="M5">
-        <v>0.6002026382373998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -626,11 +608,8 @@
       <c r="L6">
         <v>0.6958156690267143</v>
       </c>
-      <c r="M6">
-        <v>0.7684421571265303</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -667,11 +646,8 @@
       <c r="L7">
         <v>0.6717235072144493</v>
       </c>
-      <c r="M7">
-        <v>0.7733781645198237</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -708,11 +684,8 @@
       <c r="L8">
         <v>0.76685936894059</v>
       </c>
-      <c r="M8">
-        <v>0.792688399776082</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -749,11 +722,8 @@
       <c r="L9">
         <v>0.5106134079192567</v>
       </c>
-      <c r="M9">
-        <v>0.5142328071377197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -790,11 +760,8 @@
       <c r="L10">
         <v>0.7153713701422201</v>
       </c>
-      <c r="M10">
-        <v>0.7768685428215618</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -831,11 +798,8 @@
       <c r="L11">
         <v>0.7764655754886295</v>
       </c>
-      <c r="M11">
-        <v>0.852238089874453</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -870,50 +834,6 @@
         <v>0.7764655754886295</v>
       </c>
       <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>0.7678977426220139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>0.6129792080926055</v>
-      </c>
-      <c r="C13">
-        <v>0.7873734238037797</v>
-      </c>
-      <c r="D13">
-        <v>0.7998627534245836</v>
-      </c>
-      <c r="E13">
-        <v>0.6002026382373998</v>
-      </c>
-      <c r="F13">
-        <v>0.7684421571265303</v>
-      </c>
-      <c r="G13">
-        <v>0.7733781645198237</v>
-      </c>
-      <c r="H13">
-        <v>0.792688399776082</v>
-      </c>
-      <c r="I13">
-        <v>0.5142328071377198</v>
-      </c>
-      <c r="J13">
-        <v>0.7768685428215618</v>
-      </c>
-      <c r="K13">
-        <v>0.852238089874453</v>
-      </c>
-      <c r="L13">
-        <v>0.7678977426220139</v>
-      </c>
-      <c r="M13">
         <v>1</v>
       </c>
     </row>

</xml_diff>